<commit_message>
Nova função de Notificação de Pendências. Através da Data_Ultimo_Atendimento no banco de dados e a função relativedelta da biblioteca, podemos comparar a data do ultimo atendimento com o Intervalo_Servico que é salvo sempre que um serviço exige uma nova intervenção a cada certo tempo determinado pelo Usuário. Assim a função exibe nas notificações do Sistema Operacional quantas tarefas estão pendentes. Nas próximas atualizações, precisa criar uma aba só para essas pendencias e modificar as tarefas pendentes que foram concluidas e não precisam mais de intervenção.
</commit_message>
<xml_diff>
--- a/Novo Banco de dados (database)/TesteBancodeDados/Planilhas/Dados_Atendimento.xlsx
+++ b/Novo Banco de dados (database)/TesteBancodeDados/Planilhas/Dados_Atendimento.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>ID_Cliente</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Serviço</t>
+          <t>ID_Servico</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -456,35 +456,55 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Funcionário</t>
+          <t>ID_Funcionario</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Valor Total do Serviço</t>
+          <t>Valor_Total</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Data_Ultimo_Atendimento</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Execucao</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-02-04</t>
+          <t>2025-02-06</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Andamento</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implantação do Sistema de Pendências. Agora, após concluir um pedido que estava anteriormente pendente, é possível conclui-lo através da nova função Concluir_Pendencias(). Ele irá alterar o Atendimento no banco de dados, na coluna Execucao para 'Concluido'. Assim, o Atendimento em questão, não irá passar novamente para verificações futuras. Com isso, várias das funções básicas estão concluídas.
</commit_message>
<xml_diff>
--- a/Novo Banco de dados (database)/TesteBancodeDados/Planilhas/Dados_Atendimento.xlsx
+++ b/Novo Banco de dados (database)/TesteBancodeDados/Planilhas/Dados_Atendimento.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,39 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Andamento</t>
+          <t>Concluido</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Concluido</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Substituição do SQLite pelo PostegreSQL, onde tem uma aplicação mais robusta para o ERP. Futuramente, vários usuários poderão acessar o ERP de dispositívos diferentes, e o Postegre tem uma escalabilidade muito maior que o SQLite, que não aceita o acesso de vários usuários ao mesmo tempo. Também possuigurança. recursos mais avancados, como o suporte ao JSON e permissões específicas a certos usuários, para evitar acessos indevidos a várias partes do banco de dados. Permite a criptografia dos seus dados para uma maior segurança.
</commit_message>
<xml_diff>
--- a/Novo Banco de dados (database)/TesteBancodeDados/Planilhas/Dados_Atendimento.xlsx
+++ b/Novo Banco de dados (database)/TesteBancodeDados/Planilhas/Dados_Atendimento.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,42 +440,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID_Atendimento</t>
+          <t>id_atendimento</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ID_Cliente</t>
+          <t>id_cliente</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ID_Servico</t>
+          <t>id_servico</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Data</t>
+          <t>data</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ID_Funcionario</t>
+          <t>id_funcionario</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Valor_Total</t>
+          <t>valor_total</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Data_Ultimo_Atendimento</t>
+          <t>data_ultimo_atendimento</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Execucao</t>
+          <t>execucao</t>
         </is>
       </c>
     </row>
@@ -480,30 +484,30 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-02-06</t>
-        </is>
+      <c r="D2" s="2" t="n">
+        <v>45700</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" t="n">
-        <v>50</v>
+        <v>2</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>100.20</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-02-06</t>
+          <t>2025-02-12</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Concluido</t>
+          <t>Andamento</t>
         </is>
       </c>
     </row>
@@ -515,27 +519,59 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45700</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>150.00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-02-12</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Andamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-02-06</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>34</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2025-02-06</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Concluido</t>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45700</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>150.00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-02-12</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Andamento</t>
         </is>
       </c>
     </row>

</xml_diff>